<commit_message>
finalised pc layout, fixed condition unit bug
</commit_message>
<xml_diff>
--- a/unit interface.xlsx
+++ b/unit interface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0641CB67-9BFD-476E-AAE5-AF8731A33FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4906AC6B-0B50-48FB-98C7-20F1677E2BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,6 +413,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -430,27 +451,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -774,10 +774,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -797,9 +797,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="14" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -814,9 +814,9 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
@@ -829,9 +829,9 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="14"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
@@ -844,9 +844,9 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="14"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
@@ -859,8 +859,8 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -878,9 +878,9 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="14" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -895,9 +895,9 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="14"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
@@ -910,9 +910,9 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="14"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="2" t="s">
         <v>23</v>
       </c>
@@ -925,9 +925,9 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="2" t="s">
         <v>24</v>
       </c>
@@ -940,8 +940,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -959,9 +959,9 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="14" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -976,9 +976,9 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="14"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="2" t="s">
         <v>28</v>
       </c>
@@ -991,9 +991,9 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1006,9 +1006,9 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="14"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1021,8 +1021,8 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1040,9 +1040,9 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="14" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1057,9 +1057,9 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="14"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1072,9 +1072,9 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="14"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1087,9 +1087,9 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="14"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1102,11 +1102,11 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="14"/>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1121,9 +1121,9 @@
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="14"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="20"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="2" t="s">
         <v>48</v>
       </c>
@@ -1136,9 +1136,9 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="14"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="19" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="13" t="s">
         <v>57</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1153,9 +1153,9 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="14"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="20"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="2" t="s">
         <v>49</v>
       </c>
@@ -1168,9 +1168,9 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="14"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="19" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="13" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -1185,9 +1185,9 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="14"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="20"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="2" t="s">
         <v>54</v>
       </c>
@@ -1200,8 +1200,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="14"/>
-      <c r="B28" s="9"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="4" t="s">
         <v>74</v>
       </c>
@@ -1219,8 +1219,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="14"/>
-      <c r="B29" s="10"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="4" t="s">
         <v>75</v>
       </c>
@@ -1238,7 +1238,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" s="14"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="2" t="s">
         <v>37</v>
       </c>
@@ -1255,7 +1255,7 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A31" s="14"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
         <v>38</v>
       </c>
@@ -1272,7 +1272,7 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="14"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
         <v>39</v>
       </c>
@@ -1289,7 +1289,7 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="17"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1306,10 +1306,10 @@
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="18" t="s">
         <v>65</v>
       </c>
       <c r="C34" s="5" t="s">
@@ -1329,9 +1329,9 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="13"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="14" t="s">
+      <c r="A35" s="20"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="9" t="s">
         <v>67</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -1348,9 +1348,9 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="13"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="14"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="9"/>
       <c r="D36" s="2" t="s">
         <v>61</v>
       </c>
@@ -1363,9 +1363,9 @@
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="13"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="14" t="s">
+      <c r="A37" s="20"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -1380,9 +1380,9 @@
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="13"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="14"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="9"/>
       <c r="D38" s="2" t="s">
         <v>63</v>
       </c>
@@ -1395,11 +1395,11 @@
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="13"/>
-      <c r="B39" s="15" t="s">
+      <c r="A39" s="20"/>
+      <c r="B39" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="8" t="s">
         <v>56</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -1414,9 +1414,9 @@
       <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A40" s="13"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
+      <c r="A40" s="20"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
       <c r="D40" s="2" t="s">
         <v>48</v>
       </c>
@@ -1429,9 +1429,9 @@
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A41" s="13"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15" t="s">
+      <c r="A41" s="20"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8" t="s">
         <v>57</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -1446,9 +1446,9 @@
       <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A42" s="13"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
       <c r="D42" s="2" t="s">
         <v>49</v>
       </c>
@@ -1461,8 +1461,8 @@
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="13"/>
-      <c r="B43" s="14" t="s">
+      <c r="A43" s="20"/>
+      <c r="B43" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1480,8 +1480,8 @@
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A44" s="13"/>
-      <c r="B44" s="14"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="2" t="s">
         <v>68</v>
       </c>
@@ -1497,7 +1497,7 @@
       <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A45" s="13"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="2" t="s">
         <v>38</v>
       </c>
@@ -1514,7 +1514,7 @@
       <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="13"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="2" t="s">
         <v>39</v>
       </c>
@@ -1531,7 +1531,7 @@
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A47" s="11"/>
+      <c r="A47" s="18"/>
       <c r="B47" s="2" t="s">
         <v>70</v>
       </c>
@@ -1549,6 +1549,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="A34:A47"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B43:B44"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="C18:C21"/>
     <mergeCell ref="A2:A33"/>
@@ -1562,14 +1570,6 @@
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="B22:B29"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="A34:A47"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B43:B44"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added memory interface to schematics
</commit_message>
<xml_diff>
--- a/unit interface.xlsx
+++ b/unit interface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4906AC6B-0B50-48FB-98C7-20F1677E2BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC2F062-9065-4949-8B1B-C0C37632E57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="106">
   <si>
     <t>Unit</t>
   </si>
@@ -271,6 +271,78 @@
   </si>
   <si>
     <t>normal operation on high, 0 to PC on low</t>
+  </si>
+  <si>
+    <t>memory unit</t>
+  </si>
+  <si>
+    <t>OP0-OP4</t>
+  </si>
+  <si>
+    <t>OP_CD0-OP_CD2</t>
+  </si>
+  <si>
+    <t>AD_RGC0-AD_RGC2</t>
+  </si>
+  <si>
+    <t>opcode</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>MODEB</t>
+  </si>
+  <si>
+    <t>MODEA</t>
+  </si>
+  <si>
+    <t>WD_OUT0-WD_OUT2</t>
+  </si>
+  <si>
+    <t>output address</t>
+  </si>
+  <si>
+    <t>value mode</t>
+  </si>
+  <si>
+    <t>high for register address, low for immediate</t>
+  </si>
+  <si>
+    <t>bus A/B source</t>
+  </si>
+  <si>
+    <t>WD_A0-WD_A7</t>
+  </si>
+  <si>
+    <t>WD_B0-WD_B7</t>
+  </si>
+  <si>
+    <t>instruction word</t>
+  </si>
+  <si>
+    <t>PAGE0-PAGE7</t>
+  </si>
+  <si>
+    <t>MODEMEM</t>
+  </si>
+  <si>
+    <t>high for ram, low for program memory</t>
+  </si>
+  <si>
+    <t>MEMOUT0-MEMOUT7</t>
+  </si>
+  <si>
+    <t>memory input</t>
+  </si>
+  <si>
+    <t>memory output</t>
+  </si>
+  <si>
+    <t>memory mode</t>
+  </si>
+  <si>
+    <t>memory control</t>
   </si>
 </sst>
 </file>
@@ -308,7 +380,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -398,11 +470,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -413,11 +498,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -443,15 +534,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -732,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -744,7 +838,7 @@
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.3984375" customWidth="1"/>
     <col min="3" max="3" width="15.46484375" customWidth="1"/>
-    <col min="4" max="4" width="15.265625" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" customWidth="1"/>
     <col min="5" max="5" width="8.46484375" customWidth="1"/>
     <col min="6" max="6" width="10.53125" customWidth="1"/>
     <col min="7" max="7" width="49.1328125" customWidth="1"/>
@@ -774,10 +868,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -797,9 +891,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="9"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -814,9 +908,9 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="9"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
@@ -829,9 +923,9 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="9"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
@@ -844,9 +938,9 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="9"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
@@ -859,8 +953,8 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="9"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -878,9 +972,9 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="9"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -895,9 +989,9 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="9"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
@@ -910,9 +1004,9 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="9"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="2" t="s">
         <v>23</v>
       </c>
@@ -925,9 +1019,9 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="2" t="s">
         <v>24</v>
       </c>
@@ -940,8 +1034,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -959,9 +1053,9 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -976,9 +1070,9 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="2" t="s">
         <v>28</v>
       </c>
@@ -991,9 +1085,9 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1006,9 +1100,9 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1021,8 +1115,8 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="9"/>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1040,9 +1134,9 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1057,9 +1151,9 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="9"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1072,9 +1166,9 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1087,9 +1181,9 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="9"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1102,11 +1196,11 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="9"/>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="10"/>
+      <c r="B22" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="15" t="s">
         <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1121,9 +1215,9 @@
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="9"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="14"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="2" t="s">
         <v>48</v>
       </c>
@@ -1136,9 +1230,9 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="9"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="13" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="15" t="s">
         <v>57</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1153,9 +1247,9 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="9"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="14"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="2" t="s">
         <v>49</v>
       </c>
@@ -1168,9 +1262,9 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="9"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="13" t="s">
+      <c r="A26" s="10"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="15" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -1185,9 +1279,9 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="9"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="14"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="2" t="s">
         <v>54</v>
       </c>
@@ -1200,8 +1294,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="9"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="4" t="s">
         <v>74</v>
       </c>
@@ -1219,8 +1313,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="9"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="4" t="s">
         <v>75</v>
       </c>
@@ -1238,7 +1332,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" s="9"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="2" t="s">
         <v>37</v>
       </c>
@@ -1255,7 +1349,7 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A31" s="9"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="2" t="s">
         <v>38</v>
       </c>
@@ -1272,7 +1366,7 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="9"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="2" t="s">
         <v>39</v>
       </c>
@@ -1289,7 +1383,7 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="11"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1309,7 +1403,7 @@
       <c r="A34" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="8" t="s">
         <v>65</v>
       </c>
       <c r="C34" s="5" t="s">
@@ -1330,8 +1424,8 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="20"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="9" t="s">
+      <c r="B35" s="9"/>
+      <c r="C35" s="10" t="s">
         <v>67</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -1349,8 +1443,8 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="20"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
       <c r="D36" s="2" t="s">
         <v>61</v>
       </c>
@@ -1364,8 +1458,8 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="20"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="9" t="s">
+      <c r="B37" s="9"/>
+      <c r="C37" s="10" t="s">
         <v>66</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -1381,8 +1475,8 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="20"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
       <c r="D38" s="2" t="s">
         <v>63</v>
       </c>
@@ -1396,10 +1490,10 @@
     </row>
     <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="20"/>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="11" t="s">
         <v>56</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -1415,8 +1509,8 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="20"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="2" t="s">
         <v>48</v>
       </c>
@@ -1430,8 +1524,8 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="20"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8" t="s">
+      <c r="B41" s="11"/>
+      <c r="C41" s="11" t="s">
         <v>57</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -1447,8 +1541,8 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="20"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="2" t="s">
         <v>49</v>
       </c>
@@ -1462,7 +1556,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="20"/>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1481,7 +1575,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="20"/>
-      <c r="B44" s="9"/>
+      <c r="B44" s="10"/>
       <c r="C44" s="2" t="s">
         <v>68</v>
       </c>
@@ -1530,33 +1624,272 @@
       </c>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A47" s="18"/>
-      <c r="B47" s="2" t="s">
+    <row r="47" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A47" s="23"/>
+      <c r="B47" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G47" s="2"/>
+      <c r="E47" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49" s="10"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" s="10"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A52" s="10"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A53" s="10"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A54" s="10"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A56" s="10"/>
+      <c r="B56" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A61" s="13"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E61" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F61" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G61" s="25" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="A34:A47"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B43:B44"/>
+  <mergeCells count="28">
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="B56:B61"/>
+    <mergeCell ref="A48:A61"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="B48:B55"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="C18:C21"/>
     <mergeCell ref="A2:A33"/>
@@ -1570,6 +1903,14 @@
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="B22:B29"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="A34:A47"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B43:B44"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>